<commit_message>
Update EV prices and subsidy file
</commit_message>
<xml_diff>
--- a/InputData/trans/BESP/BAU EV Subsidy Perc.xlsx
+++ b/InputData/trans/BESP/BAU EV Subsidy Perc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-2.0.0-us\InputData\trans\BESP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\trans\BESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="16" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -537,10 +537,10 @@
     <t>Subsidy Percentage (dimensionless)</t>
   </si>
   <si>
-    <t>New Vehicle Price after Carbon Tax[LDVs,passenger,battery electric vehicle] : MostRecentRun</t>
-  </si>
-  <si>
     <t>New Vehicles[LDVs,passenger,plugin hybrid vehicle] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>New Vehicle Price after RnD[LDVs,passenger,battery electric vehicle] : MostRecentRun</t>
   </si>
 </sst>
 </file>
@@ -1681,7 +1681,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G22:J40" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -1908,7 +1908,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A22:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -2326,19 +2326,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="70.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="70.86328125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2346,150 +2346,150 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="20" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" s="20" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" s="20" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B23" s="3">
         <v>2017</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B29" s="3">
         <v>2017</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B30" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -2509,23 +2509,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:AF33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="3" max="3" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A2" s="6">
         <v>2019</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <f>BAU!C92</f>
         <v>2745.8606136031603</v>
@@ -2753,25 +2753,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>2500</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>39250017</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>5000</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>5540545</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>3500</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>952065</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>1500</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>4681666</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>2500</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>6811779</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>1500</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>3923561</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>2500</v>
       </c>
@@ -2859,15 +2859,15 @@
         <v>1056426</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>323127513</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
         <v>24</v>
@@ -2885,29 +2885,29 @@
         <v>260911454</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f>SUMPRODUCT(A9:A15,C9:C15)/C18</f>
         <v>500.54031765472104</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f>A3+$A$22</f>
         <v>3246.4009312578814</v>
@@ -3135,220 +3135,220 @@
         <v>500.54031765472104</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>71</v>
       </c>
       <c r="B28">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C28">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D28">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E28">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F28">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G28">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="H28">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="I28">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="J28">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="K28">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="L28">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="M28">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="N28">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="O28">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="P28">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="Q28">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="R28">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="S28">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="T28">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="U28">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="V28">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="W28">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="X28">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="Y28">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="Z28">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="AA28">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="AB28">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="AC28">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="AD28">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="AE28">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="AF28">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="AG28">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="AH28">
         <v>2050</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B29">
-        <v>53703</v>
+        <v>39357</v>
       </c>
       <c r="C29">
-        <v>51776.5</v>
+        <v>36818.400000000001</v>
       </c>
       <c r="D29">
-        <v>50407.6</v>
+        <v>35452.699999999997</v>
       </c>
       <c r="E29">
-        <v>49301.3</v>
+        <v>34556.1</v>
       </c>
       <c r="F29">
-        <v>48343.4</v>
+        <v>33882.300000000003</v>
       </c>
       <c r="G29">
-        <v>47462.2</v>
+        <v>33343.5</v>
       </c>
       <c r="H29">
-        <v>46667.199999999997</v>
+        <v>32898.800000000003</v>
       </c>
       <c r="I29">
-        <v>45962.6</v>
+        <v>32501.200000000001</v>
       </c>
       <c r="J29">
-        <v>45330.9</v>
+        <v>32141</v>
       </c>
       <c r="K29">
-        <v>44750.2</v>
+        <v>31816.799999999999</v>
       </c>
       <c r="L29">
-        <v>44223.9</v>
+        <v>31525.3</v>
       </c>
       <c r="M29">
-        <v>43738.9</v>
+        <v>31263.8</v>
       </c>
       <c r="N29">
-        <v>43295.4</v>
+        <v>31031.599999999999</v>
       </c>
       <c r="O29">
-        <v>42905</v>
+        <v>30826.799999999999</v>
       </c>
       <c r="P29">
-        <v>42563.199999999997</v>
+        <v>30648.5</v>
       </c>
       <c r="Q29">
-        <v>42259.5</v>
+        <v>30492.5</v>
       </c>
       <c r="R29">
-        <v>41992</v>
+        <v>30356</v>
       </c>
       <c r="S29">
-        <v>41757.9</v>
+        <v>30234.7</v>
       </c>
       <c r="T29">
-        <v>41553.699999999997</v>
+        <v>30127.7</v>
       </c>
       <c r="U29">
-        <v>41372.699999999997</v>
+        <v>30032.6</v>
       </c>
       <c r="V29">
-        <v>41211.300000000003</v>
+        <v>29947.1</v>
       </c>
       <c r="W29">
-        <v>41067.5</v>
+        <v>29869.4</v>
       </c>
       <c r="X29">
-        <v>40939.800000000003</v>
+        <v>29799.5</v>
       </c>
       <c r="Y29">
-        <v>40826.300000000003</v>
+        <v>29736.2</v>
       </c>
       <c r="Z29">
-        <v>40724.300000000003</v>
+        <v>29678.400000000001</v>
       </c>
       <c r="AA29">
-        <v>40632.300000000003</v>
+        <v>29625.5</v>
       </c>
       <c r="AB29">
-        <v>40548.800000000003</v>
+        <v>29576.799999999999</v>
       </c>
       <c r="AC29">
-        <v>40472.800000000003</v>
+        <v>29531.7</v>
       </c>
       <c r="AD29">
-        <v>40403.199999999997</v>
+        <v>29489.9</v>
       </c>
       <c r="AE29">
-        <v>40339.300000000003</v>
+        <v>29451</v>
       </c>
       <c r="AF29">
-        <v>40280.300000000003</v>
+        <v>29414.5</v>
       </c>
       <c r="AG29">
-        <v>40225.5</v>
+        <v>29380.400000000001</v>
       </c>
       <c r="AH29">
         <v>40174.6</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>2019</v>
       </c>
@@ -3446,137 +3446,137 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A33" s="10">
-        <f>A26/C29</f>
-        <v>6.2700277756470246E-2</v>
+        <f>A26/B29</f>
+        <v>8.2485985498332734E-2</v>
       </c>
       <c r="B33" s="10">
-        <f>B26/D29</f>
-        <v>6.4403005325742169E-2</v>
+        <f t="shared" ref="B33:AF33" si="1">B26/C29</f>
+        <v>8.817332994529585E-2</v>
       </c>
       <c r="C33" s="10">
-        <f t="shared" ref="C33:AF33" si="1">C26/E29</f>
-        <v>6.5848181107960257E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.1569920803151295E-2</v>
       </c>
       <c r="D33" s="10">
         <f t="shared" si="1"/>
-        <v>4.9925866788600545E-2</v>
+        <v>6.9845444031821649E-2</v>
       </c>
       <c r="E33" s="10">
         <f t="shared" si="1"/>
-        <v>4.282252971098393E-2</v>
+        <v>5.998564057483291E-2</v>
       </c>
       <c r="F33" s="10">
         <f t="shared" si="1"/>
-        <v>3.4970441754758275E-2</v>
+        <v>4.8944249987483472E-2</v>
       </c>
       <c r="G33" s="10">
         <f t="shared" si="1"/>
-        <v>3.1193371498232918E-2</v>
+        <v>4.357996209055285E-2</v>
       </c>
       <c r="H33" s="10">
         <f t="shared" si="1"/>
-        <v>3.1628060700861452E-2</v>
+        <v>4.4113092957327127E-2</v>
       </c>
       <c r="I33" s="10">
         <f t="shared" si="1"/>
-        <v>2.7810996969038583E-2</v>
+        <v>3.8721498290777208E-2</v>
       </c>
       <c r="J33" s="10">
         <f t="shared" si="1"/>
-        <v>2.814197021438342E-2</v>
+        <v>3.9116054303508556E-2</v>
       </c>
       <c r="K33" s="10">
         <f t="shared" si="1"/>
-        <v>2.5662804338246789E-2</v>
+        <v>3.5605143572627146E-2</v>
       </c>
       <c r="L33" s="10">
         <f t="shared" si="1"/>
-        <v>1.7110063830100854E-2</v>
+        <v>2.3694722252245365E-2</v>
       </c>
       <c r="M33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2095037653643292E-2</v>
+        <v>1.6722875730853886E-2</v>
       </c>
       <c r="N33" s="10">
         <f t="shared" si="1"/>
-        <v>1.219216578005332E-2</v>
+        <v>1.6833975324378966E-2</v>
       </c>
       <c r="O33" s="10">
         <f t="shared" si="1"/>
-        <v>1.227978538623423E-2</v>
+        <v>1.6931908267274597E-2</v>
       </c>
       <c r="P33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2358010824194262E-2</v>
+        <v>1.7018532115423972E-2</v>
       </c>
       <c r="Q33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2427291375513745E-2</v>
+        <v>1.7095058325522647E-2</v>
       </c>
       <c r="R33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2488360616011702E-2</v>
+        <v>1.7163642785592893E-2</v>
       </c>
       <c r="S33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2542995514664633E-2</v>
+        <v>1.7224600302365115E-2</v>
       </c>
       <c r="T33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2145705611196954E-2</v>
+        <v>1.6666566253162266E-2</v>
       </c>
       <c r="U33" s="10">
         <f t="shared" si="1"/>
-        <v>1.218823443488698E-2</v>
+        <v>1.6714149872766346E-2</v>
       </c>
       <c r="V33" s="10">
         <f t="shared" si="1"/>
-        <v>1.222625214717026E-2</v>
+        <v>1.6757628799196535E-2</v>
       </c>
       <c r="W33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2260241992409819E-2</v>
+        <v>1.6796936782654776E-2</v>
       </c>
       <c r="X33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2290949571993158E-2</v>
+        <v>1.6832692733258488E-2</v>
       </c>
       <c r="Y33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2318778844779178E-2</v>
+        <v>1.6865475148751988E-2</v>
       </c>
       <c r="Z33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2344146254752816E-2</v>
+        <v>1.6895590543778875E-2</v>
       </c>
       <c r="AA33" s="10">
         <f t="shared" si="1"/>
-        <v>1.236732614631854E-2</v>
+        <v>1.6923410161164189E-2</v>
       </c>
       <c r="AB33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2388630545469693E-2</v>
+        <v>1.6949255127700777E-2</v>
       </c>
       <c r="AC33" s="10">
         <f t="shared" si="1"/>
-        <v>1.240825491901746E-2</v>
+        <v>1.6973279585713107E-2</v>
       </c>
       <c r="AD33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2426429735000013E-2</v>
+        <v>1.6995698538410275E-2</v>
       </c>
       <c r="AE33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2443358507780413E-2</v>
+        <v>1.7016788238954292E-2</v>
       </c>
       <c r="AF33" s="10">
         <f t="shared" si="1"/>
-        <v>1.2459123865694271E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+        <v>1.7036538564986214E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.45">
       <c r="B45" s="13"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
@@ -3598,30 +3598,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI92"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" customWidth="1"/>
+    <col min="6" max="6" width="11.86328125" customWidth="1"/>
+    <col min="7" max="7" width="13.1328125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
+    <col min="10" max="10" width="11.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>44</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>10491284.759464676</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>2742926.6364013483</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>10044622.790505566</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>520525.68376530847</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>5294154.9930739682</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>21619399.202694658</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>1758815.7387046153</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>3203277.9124866971</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>4962634.4062189991</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>1820215.3292029649</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>8707283.6971664578</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>2272815.2177190986</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>103198947.36781919</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>13285904.130782969</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>2712962.9636383313</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>2289597.9928575293</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>2235598.1774976109</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>3255</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>8256</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
@@ -6289,7 +6289,7 @@
         <v>3954</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>52</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>67</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>53</v>
       </c>
@@ -6361,7 +6361,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>54</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>2685</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>56</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>68</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>29900</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>4148</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>59</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>58</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>69</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
@@ -6611,12 +6611,12 @@
       <c r="AG43" s="17"/>
       <c r="AH43" s="17"/>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>71</v>
       </c>
@@ -6720,9 +6720,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B46">
         <v>46797</v>
@@ -6824,7 +6824,7 @@
         <v>1226380</v>
       </c>
     </row>
-    <row r="47" spans="1:34" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="22" t="s">
         <v>72</v>
       </c>
@@ -6928,12 +6928,12 @@
         <v>10120000</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>605864.72575437836</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -7207,7 +7207,7 @@
         <v>158194.03242970258</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>576599.85300218244</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>27832.326533556985</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -7618,7 +7618,7 @@
         <v>299913.78334505705</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>1239561.7780423139</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>101301.4826037552</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>184696.13747452336</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>286202.26953808416</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -8303,7 +8303,7 @@
         <v>104985.17288025538</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -8440,7 +8440,7 @@
         <v>496479.58948830335</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>56</v>
       </c>
@@ -8577,7 +8577,7 @@
         <v>130975.65427556229</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -8714,7 +8714,7 @@
         <v>5952741.1620944031</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>57</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>763444.80980466434</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>58</v>
       </c>
@@ -8988,7 +8988,7 @@
         <v>156249.8625615497</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>59</v>
       </c>
@@ -9125,7 +9125,7 @@
         <v>131998.90157459013</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>60</v>
       </c>
@@ -9262,12 +9262,12 @@
         <v>129338.45859711803</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -9275,7 +9275,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>5366</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>46</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>47</v>
       </c>
@@ -9650,7 +9650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -9783,7 +9783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>49</v>
       </c>
@@ -9916,7 +9916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>50</v>
       </c>
@@ -10049,7 +10049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>51</v>
       </c>
@@ -10182,7 +10182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -10315,7 +10315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>54</v>
       </c>
@@ -10581,7 +10581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -10714,7 +10714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -10847,7 +10847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>56</v>
       </c>
@@ -10980,7 +10980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -11113,7 +11113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>57</v>
       </c>
@@ -11246,7 +11246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>58</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>59</v>
       </c>
@@ -11512,7 +11512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>60</v>
       </c>
@@ -11645,7 +11645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -11653,7 +11653,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.45">
       <c r="C92" s="18">
         <f>SUMPRODUCT(C73:C89,C50:C66)/SUM(C50:C66)</f>
         <v>2745.8606136031603</v>
@@ -11802,12 +11802,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -11857,7 +11857,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -11889,7 +11889,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -11921,7 +11921,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -11953,7 +11953,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -11985,7 +11985,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -12017,7 +12017,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -12049,7 +12049,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -12081,7 +12081,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -12113,7 +12113,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -12177,7 +12177,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -12209,7 +12209,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -12241,7 +12241,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -12273,7 +12273,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -12305,7 +12305,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -12337,7 +12337,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -12392,7 +12392,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -12424,7 +12424,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -12456,7 +12456,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -12488,7 +12488,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -12552,7 +12552,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -12584,7 +12584,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -12616,7 +12616,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -12648,7 +12648,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -12680,7 +12680,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -12712,7 +12712,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -12776,7 +12776,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -12808,7 +12808,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -12840,7 +12840,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -12872,7 +12872,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -12904,7 +12904,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -12936,7 +12936,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -12965,7 +12965,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -12997,7 +12997,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -13029,7 +13029,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -13052,7 +13052,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -13084,7 +13084,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -13116,7 +13116,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -13148,7 +13148,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -13180,7 +13180,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -13212,7 +13212,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -13244,7 +13244,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -13276,7 +13276,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C48" t="s">
         <v>142</v>
       </c>
@@ -13302,7 +13302,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C49" t="s">
         <v>143</v>
       </c>
@@ -13349,7 +13349,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C50" t="s">
         <v>144</v>
       </c>
@@ -13372,7 +13372,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C51" t="s">
         <v>145</v>
       </c>
@@ -13433,13 +13433,13 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
         <v>146</v>
       </c>
@@ -13453,7 +13453,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="23"/>
       <c r="B2" t="s">
         <v>150</v>
@@ -13465,7 +13465,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="23"/>
       <c r="C3">
         <v>200000</v>
@@ -13474,13 +13474,13 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="23"/>
       <c r="D4">
         <v>200000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -13508,7 +13508,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -13522,7 +13522,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -13536,7 +13536,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -13564,7 +13564,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -13578,7 +13578,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -13606,7 +13606,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -13620,7 +13620,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -13634,7 +13634,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -13648,7 +13648,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -13662,7 +13662,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -13676,7 +13676,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -13690,7 +13690,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -13704,7 +13704,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -13737,12 +13737,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>168</v>
       </c>
@@ -13852,152 +13852,152 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="19">
         <f t="shared" ref="B2:C2" si="0">C2</f>
-        <v>6.2700277756470246E-2</v>
+        <v>8.2485985498332734E-2</v>
       </c>
       <c r="C2" s="19">
         <f t="shared" si="0"/>
-        <v>6.2700277756470246E-2</v>
+        <v>8.2485985498332734E-2</v>
       </c>
       <c r="D2" s="19">
         <f>E2</f>
-        <v>6.2700277756470246E-2</v>
+        <v>8.2485985498332734E-2</v>
       </c>
       <c r="E2" s="12">
         <f>Data!A33</f>
-        <v>6.2700277756470246E-2</v>
+        <v>8.2485985498332734E-2</v>
       </c>
       <c r="F2" s="12">
         <f>Data!B33</f>
-        <v>6.4403005325742169E-2</v>
+        <v>8.817332994529585E-2</v>
       </c>
       <c r="G2" s="12">
         <f>Data!C33</f>
-        <v>6.5848181107960257E-2</v>
+        <v>9.1569920803151295E-2</v>
       </c>
       <c r="H2" s="12">
         <f>Data!D33</f>
-        <v>4.9925866788600545E-2</v>
+        <v>6.9845444031821649E-2</v>
       </c>
       <c r="I2" s="12">
         <f>Data!E33</f>
-        <v>4.282252971098393E-2</v>
+        <v>5.998564057483291E-2</v>
       </c>
       <c r="J2" s="12">
         <f>Data!F33</f>
-        <v>3.4970441754758275E-2</v>
+        <v>4.8944249987483472E-2</v>
       </c>
       <c r="K2" s="12">
         <f>Data!G33</f>
-        <v>3.1193371498232918E-2</v>
+        <v>4.357996209055285E-2</v>
       </c>
       <c r="L2" s="12">
         <f>Data!H33</f>
-        <v>3.1628060700861452E-2</v>
+        <v>4.4113092957327127E-2</v>
       </c>
       <c r="M2" s="12">
         <f>Data!I33</f>
-        <v>2.7810996969038583E-2</v>
+        <v>3.8721498290777208E-2</v>
       </c>
       <c r="N2" s="12">
         <f>Data!J33</f>
-        <v>2.814197021438342E-2</v>
+        <v>3.9116054303508556E-2</v>
       </c>
       <c r="O2" s="12">
         <f>Data!K33</f>
-        <v>2.5662804338246789E-2</v>
+        <v>3.5605143572627146E-2</v>
       </c>
       <c r="P2" s="12">
         <f>Data!L33</f>
-        <v>1.7110063830100854E-2</v>
+        <v>2.3694722252245365E-2</v>
       </c>
       <c r="Q2" s="12">
         <f>Data!M33</f>
-        <v>1.2095037653643292E-2</v>
+        <v>1.6722875730853886E-2</v>
       </c>
       <c r="R2" s="12">
         <f>Data!N33</f>
-        <v>1.219216578005332E-2</v>
+        <v>1.6833975324378966E-2</v>
       </c>
       <c r="S2" s="12">
         <f>Data!O33</f>
-        <v>1.227978538623423E-2</v>
+        <v>1.6931908267274597E-2</v>
       </c>
       <c r="T2" s="12">
         <f>Data!P33</f>
-        <v>1.2358010824194262E-2</v>
+        <v>1.7018532115423972E-2</v>
       </c>
       <c r="U2" s="12">
         <f>Data!Q33</f>
-        <v>1.2427291375513745E-2</v>
+        <v>1.7095058325522647E-2</v>
       </c>
       <c r="V2" s="12">
         <f>Data!R33</f>
-        <v>1.2488360616011702E-2</v>
+        <v>1.7163642785592893E-2</v>
       </c>
       <c r="W2" s="12">
         <f>Data!S33</f>
-        <v>1.2542995514664633E-2</v>
+        <v>1.7224600302365115E-2</v>
       </c>
       <c r="X2" s="12">
         <f>Data!T33</f>
-        <v>1.2145705611196954E-2</v>
+        <v>1.6666566253162266E-2</v>
       </c>
       <c r="Y2" s="12">
         <f>Data!U33</f>
-        <v>1.218823443488698E-2</v>
+        <v>1.6714149872766346E-2</v>
       </c>
       <c r="Z2" s="12">
         <f>Data!V33</f>
-        <v>1.222625214717026E-2</v>
+        <v>1.6757628799196535E-2</v>
       </c>
       <c r="AA2" s="12">
         <f>Data!W33</f>
-        <v>1.2260241992409819E-2</v>
+        <v>1.6796936782654776E-2</v>
       </c>
       <c r="AB2" s="12">
         <f>Data!X33</f>
-        <v>1.2290949571993158E-2</v>
+        <v>1.6832692733258488E-2</v>
       </c>
       <c r="AC2" s="12">
         <f>Data!Y33</f>
-        <v>1.2318778844779178E-2</v>
+        <v>1.6865475148751988E-2</v>
       </c>
       <c r="AD2" s="12">
         <f>Data!Z33</f>
-        <v>1.2344146254752816E-2</v>
+        <v>1.6895590543778875E-2</v>
       </c>
       <c r="AE2" s="12">
         <f>Data!AA33</f>
-        <v>1.236732614631854E-2</v>
+        <v>1.6923410161164189E-2</v>
       </c>
       <c r="AF2" s="12">
         <f>Data!AB33</f>
-        <v>1.2388630545469693E-2</v>
+        <v>1.6949255127700777E-2</v>
       </c>
       <c r="AG2" s="12">
         <f>Data!AC33</f>
-        <v>1.240825491901746E-2</v>
+        <v>1.6973279585713107E-2</v>
       </c>
       <c r="AH2" s="12">
         <f>Data!AD33</f>
-        <v>1.2426429735000013E-2</v>
+        <v>1.6995698538410275E-2</v>
       </c>
       <c r="AI2" s="12">
         <f>Data!AE33</f>
-        <v>1.2443358507780413E-2</v>
+        <v>1.7016788238954292E-2</v>
       </c>
       <c r="AJ2" s="12">
         <f>Data!AF33</f>
-        <v>1.2459123865694271E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1.7036538564986214E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -14107,7 +14107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -14217,7 +14217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -14327,7 +14327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -14561,12 +14561,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>168</v>
       </c>
@@ -14676,7 +14676,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -14786,7 +14786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -14896,7 +14896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -15006,7 +15006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -15116,7 +15116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -15226,7 +15226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Edits to BAU EV subsidy and NDC scenario
</commit_message>
<xml_diff>
--- a/InputData/trans/BESP/BAU EV Subsidy Perc.xlsx
+++ b/InputData/trans/BESP/BAU EV Subsidy Perc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4082BD80-CE47-4B43-975B-164289148D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78548AB-632A-4C13-9FFF-BF0EE0FAA5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="22" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="173">
   <si>
     <t>BESP BAU EV Subsidy Percentage</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>Older versions of EPS</t>
+  </si>
+  <si>
+    <t>2020 to 2012 USD (see cpi.xlsx)</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -672,10 +675,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1701,140 +1708,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A22:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="23">
-        <item x="10"/>
-        <item x="5"/>
-        <item m="1" x="21"/>
-        <item x="16"/>
-        <item m="1" x="19"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item m="1" x="20"/>
-        <item x="11"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item m="1" x="18"/>
-        <item x="17"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="19">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of TOTAL" fld="15" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable5" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G22:J40" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -2050,6 +1924,139 @@
     <dataField name="Sum of JAN" fld="3" baseField="0" baseItem="0"/>
     <dataField name="Sum of FEB" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Sum of MAR" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable4" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A22:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="23">
+        <item x="10"/>
+        <item x="5"/>
+        <item m="1" x="21"/>
+        <item x="16"/>
+        <item m="1" x="19"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="13"/>
+        <item m="1" x="20"/>
+        <item x="11"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item m="1" x="18"/>
+        <item x="17"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of TOTAL" fld="15" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2384,9 +2391,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2529,30 +2538,43 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>35</v>
       </c>
+    </row>
+    <row r="40" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A40" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" s="24">
+        <v>0.88711067149387013</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2570,7 +2592,7 @@
   <dimension ref="A1:AG45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2685,131 +2707,131 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <f>BAU!C92</f>
-        <v>2745.8606136031603</v>
+        <f>BAU!C92*About!$B$40</f>
+        <v>2435.88225276207</v>
       </c>
       <c r="B3" s="2">
-        <f>BAU!D92</f>
-        <v>2745.8606136031603</v>
+        <f>BAU!D92*About!$B$40</f>
+        <v>2435.88225276207</v>
       </c>
       <c r="C3" s="2">
-        <f>BAU!E92</f>
-        <v>2745.8606136031599</v>
+        <f>BAU!E92*About!$B$40</f>
+        <v>2435.8822527620696</v>
       </c>
       <c r="D3" s="2">
-        <f>BAU!F92</f>
-        <v>1913.0458308533071</v>
+        <f>BAU!F92*About!$B$40</f>
+        <v>1697.0833716068259</v>
       </c>
       <c r="E3" s="2">
-        <f>BAU!G92</f>
-        <v>1531.911151993939</v>
+        <f>BAU!G92*About!$B$40</f>
+        <v>1358.9747307142914</v>
       </c>
       <c r="F3" s="2">
-        <f>BAU!H92</f>
-        <v>933.18813916995873</v>
+        <f>BAU!H92*About!$B$40</f>
+        <v>827.84115676917725</v>
       </c>
       <c r="G3" s="2">
-        <f>BAU!I92</f>
-        <v>933.18813916995794</v>
+        <f>BAU!I92*About!$B$40</f>
+        <v>827.84115676917656</v>
       </c>
       <c r="H3" s="2">
-        <f>BAU!J92</f>
-        <v>744.00735890915064</v>
+        <f>BAU!J92*About!$B$40</f>
+        <v>660.0168677582775</v>
       </c>
       <c r="I3" s="2">
-        <f>BAU!K92</f>
-        <v>744.00735890915098</v>
+        <f>BAU!K92*About!$B$40</f>
+        <v>660.01686775827773</v>
       </c>
       <c r="J3" s="2">
-        <f>BAU!L92</f>
-        <v>414.07391374925612</v>
+        <f>BAU!L92*About!$B$40</f>
+        <v>367.32938767419745</v>
       </c>
       <c r="K3" s="2">
-        <f>BAU!M92</f>
-        <v>154.75353065310316</v>
+        <f>BAU!M92*About!$B$40</f>
+        <v>137.28350849372154</v>
       </c>
       <c r="L3" s="2">
-        <f>BAU!N92</f>
-        <v>18.397272874844436</v>
+        <f>BAU!N92*About!$B$40</f>
+        <v>16.320417093659209</v>
       </c>
       <c r="M3" s="2">
-        <f>BAU!O92</f>
-        <v>18.397272874844436</v>
+        <f>BAU!O92*About!$B$40</f>
+        <v>16.320417093659209</v>
       </c>
       <c r="N3" s="2">
-        <f>BAU!P92</f>
-        <v>18.397272874844433</v>
+        <f>BAU!P92*About!$B$40</f>
+        <v>16.320417093659206</v>
       </c>
       <c r="O3" s="2">
-        <f>BAU!Q92</f>
-        <v>18.397272874844436</v>
+        <f>BAU!Q92*About!$B$40</f>
+        <v>16.320417093659209</v>
       </c>
       <c r="P3" s="2">
-        <f>BAU!R92</f>
-        <v>18.397272874844436</v>
+        <f>BAU!R92*About!$B$40</f>
+        <v>16.320417093659209</v>
       </c>
       <c r="Q3" s="2">
-        <f>BAU!S92</f>
+        <f>BAU!S92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="R3" s="2">
-        <f>BAU!T92</f>
+        <f>BAU!T92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="S3" s="2">
-        <f>BAU!U92</f>
+        <f>BAU!U92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="T3" s="2">
-        <f>BAU!V92</f>
+        <f>BAU!V92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="U3" s="2">
-        <f>BAU!W92</f>
+        <f>BAU!W92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="V3" s="2">
-        <f>BAU!X92</f>
+        <f>BAU!X92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="W3" s="2">
-        <f>BAU!Y92</f>
+        <f>BAU!Y92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="X3" s="2">
-        <f>BAU!Z92</f>
+        <f>BAU!Z92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="Y3" s="2">
-        <f>BAU!AA92</f>
+        <f>BAU!AA92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="Z3" s="2">
-        <f>BAU!AB92</f>
+        <f>BAU!AB92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="AA3" s="2">
-        <f>BAU!AC92</f>
+        <f>BAU!AC92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="AB3" s="2">
-        <f>BAU!AD92</f>
+        <f>BAU!AD92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="AC3" s="2">
-        <f>BAU!AE92</f>
+        <f>BAU!AE92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="AD3" s="2">
-        <f>BAU!AF92</f>
+        <f>BAU!AF92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="AE3" s="2">
-        <f>BAU!AG92</f>
+        <f>BAU!AG92*About!$B$40</f>
         <v>0</v>
       </c>
       <c r="AF3" s="2">
-        <f>BAU!AH92</f>
+        <f>BAU!AH92*About!$B$40</f>
         <v>0</v>
       </c>
     </row>
@@ -2955,8 +2977,8 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <f>SUMPRODUCT(A9:A15,C9:C15)/C18</f>
-        <v>500.54031765472104</v>
+        <f>SUMPRODUCT(A9:A15,C9:C15)/C18*About!B40</f>
+        <v>444.03465730443463</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.35">
@@ -3068,127 +3090,127 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2">
         <f>B3+$A$22</f>
-        <v>3246.4009312578814</v>
+        <v>2879.9169100665049</v>
       </c>
       <c r="D26" s="2">
-        <f>C3+$A$22</f>
-        <v>3246.400931257881</v>
+        <f t="shared" ref="C26:AG26" si="0">C3+$A$22</f>
+        <v>2879.916910066504</v>
       </c>
       <c r="E26" s="2">
-        <f>D3+$A$22</f>
-        <v>2413.5861485080281</v>
+        <f t="shared" si="0"/>
+        <v>2141.1180289112608</v>
       </c>
       <c r="F26" s="2">
-        <f>E3+$A$22</f>
-        <v>2032.4514696486601</v>
+        <f t="shared" si="0"/>
+        <v>1803.009388018726</v>
       </c>
       <c r="G26" s="2">
-        <f>F3+$A$22</f>
-        <v>1433.7284568246798</v>
+        <f t="shared" si="0"/>
+        <v>1271.8758140736118</v>
       </c>
       <c r="H26" s="2">
-        <f>G3+$A$22</f>
-        <v>1433.7284568246789</v>
+        <f t="shared" si="0"/>
+        <v>1271.8758140736113</v>
       </c>
       <c r="I26" s="2">
-        <f>H3+$A$22</f>
-        <v>1244.5476765638716</v>
+        <f t="shared" si="0"/>
+        <v>1104.0515250627122</v>
       </c>
       <c r="J26" s="2">
-        <f>I3+$A$22</f>
-        <v>1244.5476765638721</v>
+        <f t="shared" si="0"/>
+        <v>1104.0515250627122</v>
       </c>
       <c r="K26" s="2">
-        <f>J3+$A$22</f>
-        <v>914.6142314039771</v>
+        <f t="shared" si="0"/>
+        <v>811.36404497863214</v>
       </c>
       <c r="L26" s="2">
-        <f>K3+$A$22</f>
-        <v>655.29384830782419</v>
+        <f t="shared" si="0"/>
+        <v>581.3181657981562</v>
       </c>
       <c r="M26" s="2">
-        <f>L3+$A$22</f>
-        <v>518.93759052956545</v>
+        <f t="shared" si="0"/>
+        <v>460.35507439809385</v>
       </c>
       <c r="N26" s="2">
-        <f>M3+$A$22</f>
-        <v>518.93759052956545</v>
+        <f t="shared" si="0"/>
+        <v>460.35507439809385</v>
       </c>
       <c r="O26" s="2">
-        <f>N3+$A$22</f>
-        <v>518.93759052956545</v>
+        <f t="shared" si="0"/>
+        <v>460.35507439809385</v>
       </c>
       <c r="P26" s="2">
-        <f>O3+$A$22</f>
-        <v>518.93759052956545</v>
+        <f t="shared" si="0"/>
+        <v>460.35507439809385</v>
       </c>
       <c r="Q26" s="2">
-        <f>P3+$A$22</f>
-        <v>518.93759052956545</v>
+        <f t="shared" si="0"/>
+        <v>460.35507439809385</v>
       </c>
       <c r="R26" s="2">
-        <f>Q3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="S26" s="2">
-        <f>R3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="T26" s="2">
-        <f>S3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="U26" s="2">
-        <f>T3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="V26" s="2">
-        <f>U3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="W26" s="2">
-        <f>V3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="X26" s="2">
-        <f>W3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="Y26" s="2">
-        <f>X3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="Z26" s="2">
-        <f>Y3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="AA26" s="2">
-        <f>Z3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="AB26" s="2">
-        <f>AA3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="AC26" s="2">
-        <f>AB3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="AD26" s="2">
-        <f>AC3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="AE26" s="2">
-        <f>AD3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="AF26" s="2">
-        <f>AE3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
       <c r="AG26" s="2">
-        <f>AF3+$A$22</f>
-        <v>500.54031765472104</v>
+        <f t="shared" si="0"/>
+        <v>444.03465730443463</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.35">
@@ -3492,128 +3514,128 @@
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10">
-        <f>C26/C29</f>
-        <v>6.4933213282220209E-2</v>
+        <f t="shared" ref="C33:AG33" si="1">C26/C29</f>
+        <v>5.7602946437045062E-2</v>
       </c>
       <c r="D33" s="10">
-        <f>D26/D29</f>
-        <v>7.0123466238789539E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.2207275222570316E-2</v>
       </c>
       <c r="E33" s="10">
-        <f>E26/E29</f>
-        <v>5.5232194597759396E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.8997069237698448E-2</v>
       </c>
       <c r="F33" s="10">
-        <f>F26/F29</f>
-        <v>4.860021974396482E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3113773571818274E-2</v>
       </c>
       <c r="G33" s="10">
-        <f>G26/G29</f>
-        <v>3.5524908242761846E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.1514525205994584E-2</v>
       </c>
       <c r="H33" s="10">
-        <f>H26/H29</f>
-        <v>3.6583664796089828E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.2453759442965913E-2</v>
       </c>
       <c r="I33" s="10">
-        <f>I26/I29</f>
-        <v>3.2831259241305699E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.9124960431544031E-2</v>
       </c>
       <c r="J33" s="10">
-        <f>J26/J29</f>
-        <v>3.3912674504310028E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.0084295451671517E-2</v>
       </c>
       <c r="K33" s="10">
-        <f>K26/K29</f>
-        <v>2.5941866599841077E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.3013306699189422E-2</v>
       </c>
       <c r="L33" s="10">
-        <f>L26/L29</f>
-        <v>1.9180548473059E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.7015269235556095E-2</v>
       </c>
       <c r="M33" s="10">
-        <f>M26/M29</f>
-        <v>1.5663959822078438E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.3895665916017007E-2</v>
       </c>
       <c r="N33" s="10">
-        <f>N26/N29</f>
-        <v>1.596681919108844E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4164335694227681E-2</v>
       </c>
       <c r="O33" s="10">
-        <f>O26/O29</f>
-        <v>1.6241008958026978E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4407572362493275E-2</v>
       </c>
       <c r="P33" s="10">
-        <f>P26/P29</f>
-        <v>1.6486299175889792E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4625171932372432E-2</v>
       </c>
       <c r="Q33" s="10">
-        <f>Q26/Q29</f>
-        <v>1.6705648750613755E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4819759280897703E-2</v>
       </c>
       <c r="R33" s="10">
-        <f>R26/R29</f>
-        <v>1.6303182778148687E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4462727421810782E-2</v>
       </c>
       <c r="S33" s="10">
-        <f>S26/S29</f>
-        <v>1.6473270286480865E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4613613865540057E-2</v>
       </c>
       <c r="T33" s="10">
-        <f>T26/T29</f>
-        <v>1.6624496577546648E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4747768322154953E-2</v>
       </c>
       <c r="U33" s="10">
-        <f>U26/U29</f>
-        <v>1.6759592634232386E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4867613475717611E-2</v>
       </c>
       <c r="V33" s="10">
-        <f>V26/V29</f>
-        <v>1.6881231055412553E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4975520217210206E-2</v>
       </c>
       <c r="W33" s="10">
-        <f>W26/W29</f>
-        <v>1.6991429190136634E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5073278158502654E-2</v>
       </c>
       <c r="X33" s="10">
-        <f>X26/X29</f>
-        <v>1.709022837448387E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5160923969271978E-2</v>
       </c>
       <c r="Y33" s="10">
-        <f>Y26/Y29</f>
-        <v>1.7179445279198277E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5240069237521782E-2</v>
       </c>
       <c r="Z33" s="10">
-        <f>Z26/Z29</f>
-        <v>1.7260308545137711E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5311803903668498E-2</v>
       </c>
       <c r="AA33" s="10">
-        <f>AA26/AA29</f>
-        <v>1.7333949212839633E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5377131325842806E-2</v>
       </c>
       <c r="AB33" s="10">
-        <f>AB26/AB29</f>
-        <v>1.7401321686617916E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5436898166296464E-2</v>
       </c>
       <c r="AC33" s="10">
-        <f>AC26/AC29</f>
-        <v>1.7463186091098541E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.549177873969684E-2</v>
       </c>
       <c r="AD33" s="10">
-        <f>AD26/AD29</f>
-        <v>1.7520216374035103E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5542370912288179E-2</v>
       </c>
       <c r="AE33" s="10">
-        <f>AE26/AE29</f>
-        <v>1.7573053696353702E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5589243464770168E-2</v>
       </c>
       <c r="AF33" s="10">
-        <f>AF26/AF29</f>
-        <v>1.7622177075578123E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5632821338699993E-2</v>
       </c>
       <c r="AG33" s="10">
-        <f>AG26/AG29</f>
-        <v>1.7668020375877454E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5673489419612028E-2</v>
       </c>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.35">
@@ -3638,8 +3660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI92"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6655,19 +6677,19 @@
       <c r="A44" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="C44" s="25"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="26">
+      <c r="B45" s="25">
         <v>2018</v>
       </c>
-      <c r="C45" s="26">
+      <c r="C45" s="25">
         <v>2019</v>
       </c>
       <c r="D45">
@@ -6768,10 +6790,10 @@
       <c r="A46" t="s">
         <v>169</v>
       </c>
-      <c r="B46" s="26">
+      <c r="B46" s="25">
         <v>46797</v>
       </c>
-      <c r="C46" s="26">
+      <c r="C46" s="25">
         <v>54324</v>
       </c>
       <c r="D46">
@@ -6872,10 +6894,10 @@
       <c r="A47" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="26">
+      <c r="B47" s="25">
         <v>144063</v>
       </c>
-      <c r="C47" s="26">
+      <c r="C47" s="25">
         <v>202158</v>
       </c>
       <c r="D47" s="22">
@@ -11800,7 +11822,7 @@
         <v>2745.8606136031603</v>
       </c>
       <c r="E92" s="18">
-        <f t="shared" ref="D92:AH92" si="15">SUMPRODUCT(E73:E89,E50:E66)/SUM(E50:E66)</f>
+        <f t="shared" ref="E92:AH92" si="15">SUMPRODUCT(E73:E89,E50:E66)/SUM(E50:E66)</f>
         <v>2745.8606136031599</v>
       </c>
       <c r="F92" s="18">
@@ -13581,7 +13603,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>146</v>
       </c>
       <c r="B1" t="s">
@@ -13595,7 +13617,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
+      <c r="A2" s="27"/>
       <c r="B2" t="s">
         <v>150</v>
       </c>
@@ -13607,7 +13629,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
+      <c r="A3" s="27"/>
       <c r="C3">
         <v>200000</v>
       </c>
@@ -13616,7 +13638,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
+      <c r="A4" s="27"/>
       <c r="D4">
         <v>200000</v>
       </c>
@@ -13999,143 +14021,143 @@
       </c>
       <c r="B2" s="19">
         <f t="shared" ref="B2:C2" si="0">C2</f>
-        <v>6.4933213282220209E-2</v>
+        <v>5.7602946437045062E-2</v>
       </c>
       <c r="C2" s="19">
         <f t="shared" si="0"/>
-        <v>6.4933213282220209E-2</v>
+        <v>5.7602946437045062E-2</v>
       </c>
       <c r="D2" s="19">
         <f>E2</f>
-        <v>6.4933213282220209E-2</v>
+        <v>5.7602946437045062E-2</v>
       </c>
       <c r="E2" s="12">
         <f>F2</f>
-        <v>6.4933213282220209E-2</v>
+        <v>5.7602946437045062E-2</v>
       </c>
       <c r="F2" s="12">
         <f>Data!C33</f>
-        <v>6.4933213282220209E-2</v>
+        <v>5.7602946437045062E-2</v>
       </c>
       <c r="G2" s="12">
         <f>Data!D33</f>
-        <v>7.0123466238789539E-2</v>
+        <v>6.2207275222570316E-2</v>
       </c>
       <c r="H2" s="12">
         <f>Data!E33</f>
-        <v>5.5232194597759396E-2</v>
+        <v>4.8997069237698448E-2</v>
       </c>
       <c r="I2" s="12">
         <f>Data!F33</f>
-        <v>4.860021974396482E-2</v>
+        <v>4.3113773571818274E-2</v>
       </c>
       <c r="J2" s="12">
         <f>Data!G33</f>
-        <v>3.5524908242761846E-2</v>
+        <v>3.1514525205994584E-2</v>
       </c>
       <c r="K2" s="12">
         <f>Data!H33</f>
-        <v>3.6583664796089828E-2</v>
+        <v>3.2453759442965913E-2</v>
       </c>
       <c r="L2" s="12">
         <f>Data!I33</f>
-        <v>3.2831259241305699E-2</v>
+        <v>2.9124960431544031E-2</v>
       </c>
       <c r="M2" s="12">
         <f>Data!J33</f>
-        <v>3.3912674504310028E-2</v>
+        <v>3.0084295451671517E-2</v>
       </c>
       <c r="N2" s="12">
         <f>Data!K33</f>
-        <v>2.5941866599841077E-2</v>
+        <v>2.3013306699189422E-2</v>
       </c>
       <c r="O2" s="12">
         <f>Data!L33</f>
-        <v>1.9180548473059E-2</v>
+        <v>1.7015269235556095E-2</v>
       </c>
       <c r="P2" s="12">
         <f>Data!M33</f>
-        <v>1.5663959822078438E-2</v>
+        <v>1.3895665916017007E-2</v>
       </c>
       <c r="Q2" s="12">
         <f>Data!N33</f>
-        <v>1.596681919108844E-2</v>
+        <v>1.4164335694227681E-2</v>
       </c>
       <c r="R2" s="12">
         <f>Data!O33</f>
-        <v>1.6241008958026978E-2</v>
+        <v>1.4407572362493275E-2</v>
       </c>
       <c r="S2" s="12">
         <f>Data!P33</f>
-        <v>1.6486299175889792E-2</v>
+        <v>1.4625171932372432E-2</v>
       </c>
       <c r="T2" s="12">
         <f>Data!Q33</f>
-        <v>1.6705648750613755E-2</v>
+        <v>1.4819759280897703E-2</v>
       </c>
       <c r="U2" s="12">
         <f>Data!R33</f>
-        <v>1.6303182778148687E-2</v>
+        <v>1.4462727421810782E-2</v>
       </c>
       <c r="V2" s="12">
         <f>Data!S33</f>
-        <v>1.6473270286480865E-2</v>
+        <v>1.4613613865540057E-2</v>
       </c>
       <c r="W2" s="12">
         <f>Data!T33</f>
-        <v>1.6624496577546648E-2</v>
+        <v>1.4747768322154953E-2</v>
       </c>
       <c r="X2" s="12">
         <f>Data!U33</f>
-        <v>1.6759592634232386E-2</v>
+        <v>1.4867613475717611E-2</v>
       </c>
       <c r="Y2" s="12">
         <f>Data!V33</f>
-        <v>1.6881231055412553E-2</v>
+        <v>1.4975520217210206E-2</v>
       </c>
       <c r="Z2" s="12">
         <f>Data!W33</f>
-        <v>1.6991429190136634E-2</v>
+        <v>1.5073278158502654E-2</v>
       </c>
       <c r="AA2" s="12">
         <f>Data!X33</f>
-        <v>1.709022837448387E-2</v>
+        <v>1.5160923969271978E-2</v>
       </c>
       <c r="AB2" s="12">
         <f>Data!Y33</f>
-        <v>1.7179445279198277E-2</v>
+        <v>1.5240069237521782E-2</v>
       </c>
       <c r="AC2" s="12">
         <f>Data!Z33</f>
-        <v>1.7260308545137711E-2</v>
+        <v>1.5311803903668498E-2</v>
       </c>
       <c r="AD2" s="12">
         <f>Data!AA33</f>
-        <v>1.7333949212839633E-2</v>
+        <v>1.5377131325842806E-2</v>
       </c>
       <c r="AE2" s="12">
         <f>Data!AB33</f>
-        <v>1.7401321686617916E-2</v>
+        <v>1.5436898166296464E-2</v>
       </c>
       <c r="AF2" s="12">
         <f>Data!AC33</f>
-        <v>1.7463186091098541E-2</v>
+        <v>1.549177873969684E-2</v>
       </c>
       <c r="AG2" s="12">
         <f>Data!AD33</f>
-        <v>1.7520216374035103E-2</v>
+        <v>1.5542370912288179E-2</v>
       </c>
       <c r="AH2" s="12">
         <f>Data!AE33</f>
-        <v>1.7573053696353702E-2</v>
+        <v>1.5589243464770168E-2</v>
       </c>
       <c r="AI2" s="12">
         <f>Data!AF33</f>
-        <v>1.7622177075578123E-2</v>
+        <v>1.5632821338699993E-2</v>
       </c>
       <c r="AJ2" s="12">
         <f>Data!AG33</f>
-        <v>1.7668020375877454E-2</v>
+        <v>1.5673489419612028E-2</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">

</xml_diff>